<commit_message>
Added project draft files.
</commit_message>
<xml_diff>
--- a/Artifacts/ValidationResults.xlsx
+++ b/Artifacts/ValidationResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0b021fb3000abb44/GitHub/CovidPred_Repro/Artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="878" documentId="8_{93A31E34-9601-4D85-B018-C6301D18DCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD7EFAB3-6807-4B48-862B-E28FF82507C5}"/>
+  <xr:revisionPtr revIDLastSave="879" documentId="8_{93A31E34-9601-4D85-B018-C6301D18DCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F0791C5-8246-4998-ABBE-193959DFA860}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{F2D8299E-0562-4DAC-8D5A-D94B36258533}"/>
+    <workbookView xWindow="28680" yWindow="-210" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{F2D8299E-0562-4DAC-8D5A-D94B36258533}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
@@ -1245,102 +1245,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1354,21 +1258,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1383,6 +1272,117 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1754,17 +1754,17 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="80"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="90"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
@@ -1938,28 +1938,28 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
-      <c r="G9" s="79"/>
-      <c r="H9" s="79"/>
-      <c r="I9" s="80"/>
-      <c r="K9" s="81" t="s">
+      <c r="B9" s="89"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="89"/>
+      <c r="H9" s="89"/>
+      <c r="I9" s="90"/>
+      <c r="K9" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="L9" s="82"/>
-      <c r="M9" s="82"/>
-      <c r="N9" s="82"/>
-      <c r="O9" s="82"/>
-      <c r="P9" s="82"/>
-      <c r="Q9" s="82"/>
-      <c r="R9" s="82"/>
-      <c r="S9" s="83"/>
+      <c r="L9" s="92"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="92"/>
+      <c r="O9" s="92"/>
+      <c r="P9" s="92"/>
+      <c r="Q9" s="92"/>
+      <c r="R9" s="92"/>
+      <c r="S9" s="93"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
@@ -2253,28 +2253,28 @@
       <c r="I15" s="61"/>
     </row>
     <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="78" t="s">
+      <c r="A16" s="88" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="79"/>
-      <c r="C16" s="79"/>
-      <c r="D16" s="79"/>
-      <c r="E16" s="79"/>
-      <c r="F16" s="79"/>
-      <c r="G16" s="79"/>
-      <c r="H16" s="79"/>
-      <c r="I16" s="80"/>
-      <c r="K16" s="81" t="s">
+      <c r="B16" s="89"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="89"/>
+      <c r="F16" s="89"/>
+      <c r="G16" s="89"/>
+      <c r="H16" s="89"/>
+      <c r="I16" s="90"/>
+      <c r="K16" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="L16" s="82"/>
-      <c r="M16" s="82"/>
-      <c r="N16" s="82"/>
-      <c r="O16" s="82"/>
-      <c r="P16" s="82"/>
-      <c r="Q16" s="82"/>
-      <c r="R16" s="82"/>
-      <c r="S16" s="83"/>
+      <c r="L16" s="92"/>
+      <c r="M16" s="92"/>
+      <c r="N16" s="92"/>
+      <c r="O16" s="92"/>
+      <c r="P16" s="92"/>
+      <c r="Q16" s="92"/>
+      <c r="R16" s="92"/>
+      <c r="S16" s="93"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
@@ -2558,28 +2558,28 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="84" t="s">
+      <c r="A23" s="94" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="85"/>
-      <c r="C23" s="85"/>
-      <c r="D23" s="85"/>
-      <c r="E23" s="85"/>
-      <c r="F23" s="85"/>
-      <c r="G23" s="85"/>
-      <c r="H23" s="85"/>
-      <c r="I23" s="86"/>
-      <c r="K23" s="81" t="s">
+      <c r="B23" s="95"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="95"/>
+      <c r="F23" s="95"/>
+      <c r="G23" s="95"/>
+      <c r="H23" s="95"/>
+      <c r="I23" s="96"/>
+      <c r="K23" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="L23" s="82"/>
-      <c r="M23" s="82"/>
-      <c r="N23" s="82"/>
-      <c r="O23" s="82"/>
-      <c r="P23" s="82"/>
-      <c r="Q23" s="82"/>
-      <c r="R23" s="82"/>
-      <c r="S23" s="83"/>
+      <c r="L23" s="92"/>
+      <c r="M23" s="92"/>
+      <c r="N23" s="92"/>
+      <c r="O23" s="92"/>
+      <c r="P23" s="92"/>
+      <c r="Q23" s="92"/>
+      <c r="R23" s="92"/>
+      <c r="S23" s="93"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
@@ -2901,18 +2901,18 @@
       <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="87" t="s">
+      <c r="C1" s="98"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="89"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="99"/>
     </row>
     <row r="2" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
@@ -3120,50 +3120,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="112" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="108"/>
-      <c r="J1" s="90" t="s">
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="114"/>
+      <c r="J1" s="100" t="s">
         <v>124</v>
       </c>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91"/>
-      <c r="O1" s="91"/>
-      <c r="P1" s="91"/>
-      <c r="Q1" s="92"/>
+      <c r="K1" s="101"/>
+      <c r="L1" s="101"/>
+      <c r="M1" s="101"/>
+      <c r="N1" s="101"/>
+      <c r="O1" s="101"/>
+      <c r="P1" s="101"/>
+      <c r="Q1" s="102"/>
     </row>
     <row r="2" spans="1:17" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="109" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="93" t="s">
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="95"/>
+      <c r="G2" s="105"/>
       <c r="J2" s="51"/>
-      <c r="K2" s="96" t="s">
+      <c r="K2" s="106" t="s">
         <v>36</v>
       </c>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="93" t="s">
+      <c r="L2" s="107"/>
+      <c r="M2" s="107"/>
+      <c r="N2" s="108"/>
+      <c r="O2" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="94"/>
-      <c r="Q2" s="95"/>
+      <c r="P2" s="104"/>
+      <c r="Q2" s="105"/>
     </row>
     <row r="3" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
@@ -3419,7 +3419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453BF01A-9452-42BB-A9FE-93648F6F0B06}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -3435,32 +3435,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="100" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="92"/>
-      <c r="F1" s="115" t="s">
+      <c r="B1" s="117"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="102"/>
+      <c r="F1" s="118" t="s">
         <v>127</v>
       </c>
-      <c r="G1" s="116"/>
-      <c r="H1" s="117"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="120"/>
     </row>
     <row r="2" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="110"/>
-      <c r="B2" s="123"/>
-      <c r="C2" s="118" t="s">
+      <c r="A2" s="78"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="115" t="s">
         <v>128</v>
       </c>
-      <c r="D2" s="119"/>
+      <c r="D2" s="116"/>
       <c r="F2" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="124" t="s">
+      <c r="G2" s="87" t="s">
         <v>125</v>
       </c>
-      <c r="H2" s="120" t="s">
+      <c r="H2" s="83" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3468,10 +3468,10 @@
       <c r="A3" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="111" t="s">
+      <c r="B3" s="79" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="114" t="s">
+      <c r="C3" s="82" t="s">
         <v>34</v>
       </c>
       <c r="D3" s="45" t="s">
@@ -3480,10 +3480,10 @@
       <c r="F3" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="112">
+      <c r="G3" s="80">
         <v>50</v>
       </c>
-      <c r="H3" s="121">
+      <c r="H3" s="84">
         <v>100</v>
       </c>
     </row>
@@ -3491,7 +3491,7 @@
       <c r="A4" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="112">
+      <c r="B4" s="80">
         <v>50</v>
       </c>
       <c r="C4" s="18">
@@ -3503,10 +3503,10 @@
       <c r="F4" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="112">
+      <c r="G4" s="80">
         <v>53.85</v>
       </c>
-      <c r="H4" s="121">
+      <c r="H4" s="84">
         <v>76.92</v>
       </c>
     </row>
@@ -3514,7 +3514,7 @@
       <c r="A5" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="112">
+      <c r="B5" s="80">
         <v>53.85</v>
       </c>
       <c r="C5" s="18">
@@ -3526,10 +3526,10 @@
       <c r="F5" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="112">
+      <c r="G5" s="80">
         <v>66.67</v>
       </c>
-      <c r="H5" s="121">
+      <c r="H5" s="84">
         <v>33.33</v>
       </c>
     </row>
@@ -3537,7 +3537,7 @@
       <c r="A6" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="112">
+      <c r="B6" s="80">
         <v>66.67</v>
       </c>
       <c r="C6" s="18">
@@ -3549,10 +3549,10 @@
       <c r="F6" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="112">
+      <c r="G6" s="80">
         <v>75</v>
       </c>
-      <c r="H6" s="121">
+      <c r="H6" s="84">
         <v>81.25</v>
       </c>
     </row>
@@ -3560,7 +3560,7 @@
       <c r="A7" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="112">
+      <c r="B7" s="80">
         <v>75</v>
       </c>
       <c r="C7" s="18">
@@ -3572,10 +3572,10 @@
       <c r="F7" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="113">
+      <c r="G7" s="81">
         <v>80</v>
       </c>
-      <c r="H7" s="122">
+      <c r="H7" s="85">
         <v>100</v>
       </c>
     </row>
@@ -3583,7 +3583,7 @@
       <c r="A8" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="113">
+      <c r="B8" s="81">
         <v>80</v>
       </c>
       <c r="C8" s="36">
@@ -3613,8 +3613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D24131-4035-441B-BBEE-D4868AA761F3}">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3634,26 +3634,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="124" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="H1" s="105" t="s">
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="H1" s="124" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="105"/>
-      <c r="K1" s="103" t="s">
+      <c r="I1" s="124"/>
+      <c r="K1" s="122" t="s">
         <v>91</v>
       </c>
-      <c r="L1" s="103"/>
-      <c r="N1" s="104" t="s">
+      <c r="L1" s="122"/>
+      <c r="N1" s="123" t="s">
         <v>111</v>
       </c>
-      <c r="O1" s="104"/>
+      <c r="O1" s="123"/>
     </row>
     <row r="2" spans="1:15" s="68" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="65"/>
@@ -3871,13 +3871,13 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="103" t="s">
+      <c r="A12" s="122" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="103"/>
-      <c r="C12" s="103"/>
-      <c r="D12" s="103"/>
-      <c r="E12" s="103"/>
+      <c r="B12" s="122"/>
+      <c r="C12" s="122"/>
+      <c r="D12" s="122"/>
+      <c r="E12" s="122"/>
     </row>
     <row r="13" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="65"/>
@@ -4028,21 +4028,21 @@
       <c r="C26" s="70"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="102" t="s">
+      <c r="A27" s="121" t="s">
         <v>99</v>
       </c>
-      <c r="B27" s="102"/>
-      <c r="C27" s="102"/>
+      <c r="B27" s="121"/>
+      <c r="C27" s="121"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="102"/>
-      <c r="B28" s="102"/>
-      <c r="C28" s="102"/>
+      <c r="A28" s="121"/>
+      <c r="B28" s="121"/>
+      <c r="C28" s="121"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="102"/>
-      <c r="B29" s="102"/>
-      <c r="C29" s="102"/>
+      <c r="A29" s="121"/>
+      <c r="B29" s="121"/>
+      <c r="C29" s="121"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="71" t="s">
@@ -4052,26 +4052,26 @@
       <c r="C31" s="70"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="102" t="s">
+      <c r="A32" s="121" t="s">
         <v>102</v>
       </c>
-      <c r="B32" s="102"/>
-      <c r="C32" s="102"/>
+      <c r="B32" s="121"/>
+      <c r="C32" s="121"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="102"/>
-      <c r="B33" s="102"/>
-      <c r="C33" s="102"/>
+      <c r="A33" s="121"/>
+      <c r="B33" s="121"/>
+      <c r="C33" s="121"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="102"/>
-      <c r="B34" s="102"/>
-      <c r="C34" s="102"/>
+      <c r="A34" s="121"/>
+      <c r="B34" s="121"/>
+      <c r="C34" s="121"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="102"/>
-      <c r="B35" s="102"/>
-      <c r="C35" s="102"/>
+      <c r="A35" s="121"/>
+      <c r="B35" s="121"/>
+      <c r="C35" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>